<commit_message>
Update TCCpUCD to use consistent units with BTC
</commit_message>
<xml_diff>
--- a/InputData/elec/TCCpUCD/Trans Const Cost per Unit Cap Dist.xlsx
+++ b/InputData/elec/TCCpUCD/Trans Const Cost per Unit Cap Dist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\TCCpUCD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-southkorea\InputData\elec\TCCpUCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00FB9EC-098D-47C2-82FF-923B9AA82DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3325FEA3-F413-4A4D-BC54-CE03D437BF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>TCCpUCD Transmission Construction Cost per Unit Capacity Distance</t>
   </si>
@@ -53,22 +53,28 @@
     <t>Cost per Unit Capacity Distance (2012$/(circuit mile))</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>http://sites.utexas.edu/energyinstitute/files/2016/11/UTAustin_FCe_TransmissionCosts_2016.pdf</t>
-  </si>
-  <si>
-    <t>The University of Texas at Austin Energy Institute</t>
-  </si>
-  <si>
-    <t>Estimation of Transmission Costs for New Generation</t>
-  </si>
-  <si>
-    <t>Table 3</t>
-  </si>
-  <si>
-    <t>We adjust 2016 dollars to 2012 dollars using the following conversion factor:</t>
+    <t>MW-miles</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>$ / MW-mile</t>
+  </si>
+  <si>
+    <t>Americans for a Clean Energy Grid and Grid Strategies</t>
+  </si>
+  <si>
+    <t>Transmission Projects Ready To Go: Plugging Into America's Untapped Renewable Resources</t>
+  </si>
+  <si>
+    <t>https://cleanenergygrid.org/wp-content/uploads/2019/04/Transmission-Projects-Ready-to-Go-Final.pdf</t>
+  </si>
+  <si>
+    <t>Pages 11-12</t>
+  </si>
+  <si>
+    <t>We adjust 2021 dollars to 2012 dollars using the following conversion factor:</t>
   </si>
 </sst>
 </file>
@@ -230,55 +236,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>161104</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>37869</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FD2E4CF-B955-4B59-BEE8-2B8AF2EAB153}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="5610225"/>
-          <a:ext cx="6571429" cy="1847619"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -621,27 +578,27 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
-        <v>2016</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -651,12 +608,12 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>0.95661376543184151</v>
+        <v>0.84730412960844359</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -671,10 +628,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A13:B13"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -684,18 +641,35 @@
     <col min="3" max="3" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <f>17*10^6</f>
+        <v>17000000</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B13">
-        <f>AVERAGE(1.114,0.823,0.847)</f>
-        <v>0.92799999999999994</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f>33*10^9</f>
+        <v>33000000000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f>A2/A1</f>
+        <v>1941.1764705882354</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -726,8 +700,8 @@
         <v>2</v>
       </c>
       <c r="B2" s="6">
-        <f>Data!B13*1000000*About!A11</f>
-        <v>887737.5743207488</v>
+        <f>Data!A3*About!A11</f>
+        <v>1644.7668398281553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>